<commit_message>
[ELAB-428] added more Anforderungen
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EB22E4-9C31-4956-8F5A-1DE7D2F83005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E322FEF6-ADD8-4DFD-8347-E941B8319CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -117,6 +117,84 @@
   </si>
   <si>
     <t>Partnersysteme</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>Fehler-Monitoring</t>
+  </si>
+  <si>
+    <t>Fehlerübertragung</t>
+  </si>
+  <si>
+    <t>Sämtliche erfassten Fehler sollen an ein Partnersystem weitergeleitet werden.</t>
+  </si>
+  <si>
+    <t>Partnersystem "Log-Management"</t>
+  </si>
+  <si>
+    <t>Es existiert ein Partnersystem, zu dem Logmeldungen weitergeleitet werden. Dieses System soll die Logmeldungen speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Logmeldungen bieten.</t>
+  </si>
+  <si>
+    <t>Partnersystem "Error-Monitoring"</t>
+  </si>
+  <si>
+    <t>Partnersystem "Tracing"</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Partnersystem "Metriken"</t>
+  </si>
+  <si>
+    <t>A+S</t>
+  </si>
+  <si>
+    <t>Es existiert ein Partnersystem, zu dem Fehler weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Fehler bieten.</t>
+  </si>
+  <si>
+    <t>Es existiert ein Partnersystem, zu dem Metriken weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Metriken bieten.</t>
+  </si>
+  <si>
+    <t>Visualisierung "Metriken"</t>
+  </si>
+  <si>
+    <t>Visualisierung "Tracing"</t>
+  </si>
+  <si>
+    <t>Alerting "Metriken"</t>
+  </si>
+  <si>
+    <t>Es existiert ein Partnersystem, zu dem Tracingdaten weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Tracingdaten bieten.</t>
+  </si>
+  <si>
+    <t>Visualisierung "Error-Monitoring"</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Fehler weitergeleitet werden, soll diese grafisch darstellen können.</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Tracingdaten weitergeleitet werden, soll diese grafisch als Tracing-Wasserfallgraph darstellen können.</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Metriken weitergeleitet werden, soll diese grafisch darstellen können.</t>
+  </si>
+  <si>
+    <t>Alerting  "Error-Monitoring"</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Fehler weitergeleitet werden, soll bei Auftreten von bestimmten Fehlern oder Fehleranzahlen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Metriken weitergeleitet werden, soll bei Auftreten von bestimmten Metrikwerten oder Überschreitungen von Schwellen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so soll dieser automatisch erfasst werden und um weitere Attribute ergänzt werden.\par Sonstige Fehler können auch erfasst werden, aber hierbei Bedarf es einem manuellen Aufruf einer Schnittstelle</t>
   </si>
 </sst>
 </file>
@@ -169,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -180,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -460,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -472,7 +551,7 @@
     <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,39 +590,33 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="B4">
-        <v>1010</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="B5">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -555,15 +628,15 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45">
       <c r="B6">
-        <v>1100</v>
+        <v>1011</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -574,50 +647,59 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60">
+      <c r="B7">
+        <v>1020</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45">
+      <c r="B8">
+        <v>1100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="60">
-      <c r="B8">
-        <v>2010</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45">
+    <row r="9" spans="1:7" ht="30">
       <c r="B9">
-        <v>2020</v>
+        <v>1101</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -626,15 +708,15 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -643,41 +725,257 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7">
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="G12" s="2"/>
+    <row r="11" spans="1:7" ht="60">
+      <c r="B11">
+        <v>2010</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45">
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="7:7">
-      <c r="G21" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="45">
+      <c r="B14">
+        <v>4010</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45">
+      <c r="B15">
+        <v>4020</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="B16">
+        <v>4021</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="45">
+      <c r="B17">
+        <v>4021</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="45">
+      <c r="B18">
+        <v>4030</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30">
+      <c r="B19">
+        <v>4031</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="45">
+      <c r="B20">
+        <v>4030</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30">
+      <c r="B21">
+        <v>4031</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="45">
+      <c r="B22">
+        <v>4032</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="G27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[non-issue] fix duplicate anf: labels
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E322FEF6-ADD8-4DFD-8347-E941B8319CFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE551AA-8DBF-4A46-AE4B-30ED9691CF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -838,7 +838,7 @@
     </row>
     <row r="17" spans="2:7" ht="45">
       <c r="B17">
-        <v>4021</v>
+        <v>4022</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="20" spans="2:7" ht="45">
       <c r="B20">
-        <v>4030</v>
+        <v>4040</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="21" spans="2:7" ht="30">
       <c r="B21">
-        <v>4031</v>
+        <v>4041</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="22" spans="2:7" ht="45">
       <c r="B22">
-        <v>4032</v>
+        <v>4042</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
[ELAB-430] added more content to 'Konzept'
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ABD2BA-A75E-4E30-B3FD-27CFF7915BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D6FFDF-5A32-45E9-A921-330F422BC9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t>Id</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Auf Basis des Konzeptes, soll die Demo-Anwendung erweitert werden.</t>
+  </si>
+  <si>
+    <t>Anzahl Partnersysteme</t>
+  </si>
+  <si>
+    <t>Die Anzahl an zusätzlichen Partnersystemen, die für die Lösung benötigt werden, soll so gering wie möglich gehalten werden.</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -626,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1074,42 +1083,42 @@
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:10" ht="30">
+      <c r="B23" s="8">
+        <v>3100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" ht="45">
-      <c r="B24" s="8">
-        <v>5010</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="45">
       <c r="B25" s="8">
-        <v>5020</v>
+        <v>5010</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1121,19 +1130,19 @@
         <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="30">
+    <row r="26" spans="1:10" ht="45">
       <c r="B26" s="8">
-        <v>5021</v>
+        <v>5020</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1142,19 +1151,19 @@
         <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="45">
+    <row r="27" spans="1:10" ht="30">
       <c r="B27" s="8">
-        <v>5022</v>
+        <v>5021</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1163,19 +1172,19 @@
         <v>30</v>
       </c>
       <c r="F27" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="45">
       <c r="B28" s="8">
-        <v>5030</v>
+        <v>5022</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1184,16 +1193,16 @@
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:10" ht="45">
       <c r="B29" s="8">
-        <v>5031</v>
+        <v>5030</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1205,19 +1214,19 @@
         <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="45">
+    <row r="30" spans="1:10" ht="30">
       <c r="B30" s="8">
-        <v>5040</v>
+        <v>5031</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -1226,16 +1235,16 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="30">
+    <row r="31" spans="1:10" ht="45">
       <c r="B31" s="8">
-        <v>5041</v>
+        <v>5040</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -1247,19 +1256,19 @@
         <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="45">
+    <row r="32" spans="1:10" ht="30">
       <c r="B32" s="8">
-        <v>5042</v>
+        <v>5041</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -1268,19 +1277,19 @@
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="2:10" ht="45">
       <c r="B33" s="8">
-        <v>5050</v>
+        <v>5042</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1289,15 +1298,33 @@
         <v>30</v>
       </c>
       <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="2:10" ht="45">
+      <c r="B34" s="8">
+        <v>5050</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="G34" s="2"/>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" spans="2:10">
       <c r="G35" s="2"/>
@@ -1307,6 +1334,9 @@
     </row>
     <row r="37" spans="2:10">
       <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="G38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[non-issue] fix some typos based on Textidote
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D6FFDF-5A32-45E9-A921-330F422BC9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B934B92-679F-4726-AF08-EC5CB62C0D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,15 +110,9 @@
     <t>Eigenschaften</t>
   </si>
   <si>
-    <t>Daten die der Nachvollziehbarkeit dienen, sollen wenn möglich bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sollen mindestens 120s vorgehalten werden und in dieser Zeit sollen wiederholt Verbindungsversuche unternommen werden.</t>
-  </si>
-  <si>
     <t>Resilienz der Übertragung</t>
   </si>
   <si>
-    <t>Daten, die der Nachvollziehbarkeit dienen, sollen wenn möglich gruppiert an externe Systeme gesendet werden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
-  </si>
-  <si>
     <t>Batchverarbeitung</t>
   </si>
   <si>
@@ -285,6 +279,12 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Daten die der Nachvollziehbarkeit dienen sollen, wenn möglich bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sollen mindestens 120s vorgehalten werden und in dieser Zeit sollen wiederholt Verbindungsversuche unternommen werden.</t>
+  </si>
+  <si>
+    <t>Daten, die der Nachvollziehbarkeit dienen sollen, wenn möglich gruppiert an externe Systeme gesendet werden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
   </si>
 </sst>
 </file>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -687,22 +687,22 @@
     </row>
     <row r="3" spans="1:10" ht="45">
       <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -716,13 +716,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -736,13 +736,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -812,10 +812,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -833,10 +833,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -854,10 +854,10 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -875,10 +875,10 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J12" s="6"/>
     </row>
@@ -896,7 +896,7 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>16</v>
@@ -917,10 +917,10 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="6"/>
     </row>
@@ -938,10 +938,10 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -959,10 +959,10 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -980,10 +980,10 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -1001,10 +1001,10 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -1022,10 +1022,10 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -1055,10 +1055,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="J21" s="6"/>
     </row>
@@ -1076,10 +1076,10 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J22" s="6"/>
     </row>
@@ -1094,19 +1094,19 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="4"/>
@@ -1127,13 +1127,13 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J25" s="6"/>
     </row>
@@ -1148,13 +1148,13 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J26" s="6"/>
     </row>
@@ -1163,19 +1163,19 @@
         <v>5021</v>
       </c>
       <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
         <v>28</v>
       </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>30</v>
-      </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J27" s="6"/>
     </row>
@@ -1190,13 +1190,13 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J28" s="6"/>
     </row>
@@ -1211,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J29" s="6"/>
     </row>
@@ -1232,13 +1232,13 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1247,19 +1247,19 @@
         <v>5040</v>
       </c>
       <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="F31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -1268,19 +1268,19 @@
         <v>5041</v>
       </c>
       <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
         <v>28</v>
       </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>30</v>
-      </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1295,13 +1295,13 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J33" s="6"/>
     </row>
@@ -1316,13 +1316,13 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J34" s="6"/>
     </row>

</xml_diff>

<commit_message>
[non-issue] fix some typos based on Word
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B934B92-679F-4726-AF08-EC5CB62C0D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6925A124-24AD-4161-BBA1-53DD8E732A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -281,10 +281,10 @@
     <t>K</t>
   </si>
   <si>
-    <t>Daten die der Nachvollziehbarkeit dienen sollen, wenn möglich bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sollen mindestens 120s vorgehalten werden und in dieser Zeit sollen wiederholt Verbindungsversuche unternommen werden.</t>
-  </si>
-  <si>
     <t>Daten, die der Nachvollziehbarkeit dienen sollen, wenn möglich gruppiert an externe Systeme gesendet werden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
+  </si>
+  <si>
+    <t>Daten, die der Nachvollziehbarkeit dienen sollen, wenn möglich bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sollen mindestens 120s vorgehalten werden und in dieser Zeit sollen wiederholt Verbindungsversuche unternommen werden.</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1058,7 +1058,7 @@
         <v>18</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J21" s="6"/>
     </row>
@@ -1079,7 +1079,7 @@
         <v>19</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J22" s="6"/>
     </row>

</xml_diff>

<commit_message>
[ELAB-431] reduced usage of 'werden' in 'Anforderungen'
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6925A124-24AD-4161-BBA1-53DD8E732A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7ACA29-3067-4994-AFA2-F2690714C1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -98,15 +98,9 @@
     </r>
   </si>
   <si>
-    <t>Das Aufrufen von Schnittstellen soll mittels einer Logmeldung notiert werden. Hierbei sollen relevante Informationen wie Aufrufparameter mit notiert werden.</t>
-  </si>
-  <si>
     <t>Tritt ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, dass ein Nutzer einen neuen Datensatz angelegt möchte und wenn der diesen anlegt.</t>
   </si>
   <si>
-    <t>Ausgewählte Logmeldungen sollen an ein Partnersystem weitergeleitet werden. Die Auswahl könnte über die Kritikalität, also dem Log-Level, der Logmeldung erfolgen.</t>
-  </si>
-  <si>
     <t>Eigenschaften</t>
   </si>
   <si>
@@ -122,24 +116,12 @@
     <t>A</t>
   </si>
   <si>
-    <t>Partnersystem "Log-Management"</t>
-  </si>
-  <si>
     <t>Es existiert ein Partnersystem, zu dem Logmeldungen weitergeleitet werden. Dieses System soll die Logmeldungen speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Logmeldungen bieten.</t>
   </si>
   <si>
-    <t>Partnersystem "Error-Monitoring"</t>
-  </si>
-  <si>
-    <t>Partnersystem "Tracing"</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>Partnersystem "Metriken"</t>
-  </si>
-  <si>
     <t>A+S</t>
   </si>
   <si>
@@ -149,42 +131,12 @@
     <t>Es existiert ein Partnersystem, zu dem Metriken weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Metriken bieten.</t>
   </si>
   <si>
-    <t>Visualisierung "Metriken"</t>
-  </si>
-  <si>
-    <t>Visualisierung "Tracing"</t>
-  </si>
-  <si>
-    <t>Alerting "Metriken"</t>
-  </si>
-  <si>
     <t>Es existiert ein Partnersystem, zu dem Tracingdaten weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Tracingdaten bieten.</t>
   </si>
   <si>
-    <t>Visualisierung "Error-Monitoring"</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Fehler weitergeleitet werden, soll diese grafisch darstellen können.</t>
-  </si>
-  <si>
     <t>Das Partnersystem, zu dem die Tracingdaten weitergeleitet werden, soll diese grafisch als Tracing-Wasserfallgraph darstellen können.</t>
   </si>
   <si>
-    <t>Das Partnersystem, zu dem die Metriken weitergeleitet werden, soll diese grafisch darstellen können.</t>
-  </si>
-  <si>
-    <t>Alerting  "Error-Monitoring"</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Fehler weitergeleitet werden, soll bei Auftreten von bestimmten Fehlern oder Fehleranzahlen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Metriken weitergeleitet werden, soll bei Auftreten von bestimmten Metrikwerten oder Überschreitungen von Schwellen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
-  </si>
-  <si>
-    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so soll dieser automatisch erfasst werden und um weitere Attribute ergänzt werden.\par Sonstige Fehler können auch erfasst werden, aber hierbei Bedarf es einem manuellen Aufruf einer Schnittstelle</t>
-  </si>
-  <si>
     <t>Error-Monitoring</t>
   </si>
   <si>
@@ -203,9 +155,6 @@
     <t>Es existiert ein Partnersystem, zu die Session-Replay-Daten weitergeleitet werden. Dieses System soll anhand dieser Daten eine Benutzersitzung rekreieren können.</t>
   </si>
   <si>
-    <t>Partnersystem "Session-Replay"</t>
-  </si>
-  <si>
     <t>Session-Replay</t>
   </si>
   <si>
@@ -224,33 +173,15 @@
     <t>Übertragung von Session-Replay-Daten</t>
   </si>
   <si>
-    <t>Sämtlich erfasste Session-Replay-Daten sollen an ein Partnersystem weitergeleitet werden.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Fehler sollen an ein Partnersystem weitergeleitet werden.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Tracingdaten sollen an ein Partnersystem weitergeleitet werden.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Metrikdaten sollen an ein Partnersystem weitergeleitet werden.</t>
-  </si>
-  <si>
     <t>Es sollen Daten erhoben werden, anhand dessen die Benutzerinteraktionen und das Anwendungsverhalten nachgestellt werden kann. Diese Funktionalität darf jedoch standardmäßig deaktiviert sein.</t>
   </si>
   <si>
     <t>Datadump</t>
   </si>
   <si>
-    <t>Möglichkeit zum Export des fachlichen Modells des Frontends</t>
-  </si>
-  <si>
     <t>Datadump-Import</t>
   </si>
   <si>
-    <t>Re-Import des fachlichen Modells des Frontends, um diesen Zustand auf anderen Systemen und für andere Systeme einsehbar zu machen</t>
-  </si>
-  <si>
     <t>1010</t>
   </si>
   <si>
@@ -263,15 +194,9 @@
     <t>Demo-Anwendung</t>
   </si>
   <si>
-    <t>Es soll eine Demo-Anwendung erstellt werden, welche später dazu dienen soll, das Konzept darauf anwenden zu können.\par Diese Demo-Anwendung soll Fehler beinhalten, die dann mithilfe der Lösung nachvollziehbarer gemacht werden sollten.</t>
-  </si>
-  <si>
     <t>Proof-of-Concept</t>
   </si>
   <si>
-    <t>Auf Basis des Konzeptes, soll die Demo-Anwendung erweitert werden.</t>
-  </si>
-  <si>
     <t>Anzahl Partnersysteme</t>
   </si>
   <si>
@@ -281,10 +206,85 @@
     <t>K</t>
   </si>
   <si>
-    <t>Daten, die der Nachvollziehbarkeit dienen sollen, wenn möglich gruppiert an externe Systeme gesendet werden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
-  </si>
-  <si>
-    <t>Daten, die der Nachvollziehbarkeit dienen sollen, wenn möglich bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sollen mindestens 120s vorgehalten werden und in dieser Zeit sollen wiederholt Verbindungsversuche unternommen werden.</t>
+    <t>Partnersystem \textit{Log-Management}</t>
+  </si>
+  <si>
+    <t>Partnersystem \textit{Error-Monitoring}</t>
+  </si>
+  <si>
+    <t>Visualisierung \textit{Error-Monitoring}</t>
+  </si>
+  <si>
+    <t>Alerting  \textit{Error-Monitoring}</t>
+  </si>
+  <si>
+    <t>Partnersystem \textit{Tracing}</t>
+  </si>
+  <si>
+    <t>Visualisierung \textit{Tracing}</t>
+  </si>
+  <si>
+    <t>Partnersystem \textit{Metriken}</t>
+  </si>
+  <si>
+    <t>Visualisierung \textit{Metriken}</t>
+  </si>
+  <si>
+    <t>Alerting \textit{Metriken}</t>
+  </si>
+  <si>
+    <t>Partnersystem \textit{Session-Replay}</t>
+  </si>
+  <si>
+    <t>Auf Basis des Konzeptes, ist die Demo-Anwendung zu erweitern.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Tracingdaten sind an ein Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Ausgewählte Logmeldungen sind an ein Partnersystem weiterzuleiten. Die Auswahl könnte über die Kritikalität, also dem Log-Level, der Logmeldung erfolgen.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Fehler sind an ein Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Metrikdaten sind an ein Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Session-Replay-Daten sind an ein Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so ist dieser automatisch zu erfasst und um weitere Attribute zu ergänzen.\par Sonstige Fehler können auch erfasst werden, aber hierbei Bedarf es einem manuellen Aufruf einer Schnittstelle</t>
+  </si>
+  <si>
+    <t>Das Aufrufen von Schnittstellen ist mittels einer Logmeldung zu notieren. Hierbei sind relevante Informationen wie Aufrufparameter ebenfalls zu notieren.</t>
+  </si>
+  <si>
+    <t>Eine Demo-Anwendung ist zu Erstellen und soll dazu dienen, das Konzept darauf anwenden zu können.\par Diese Demo-Anwendung soll Fehlerverhalten beinhalten, die dann mithilfe der Lösung besser nachvollziehbar zu gestalten sind.</t>
+  </si>
+  <si>
+    <t>Möglichkeit zum Export des fachlichen Modells des Frontends.</t>
+  </si>
+  <si>
+    <t>Re-Import des fachlichen Modells des Frontends, um diesen Zustand auf anderen Systemen und für andere Systeme einsehbar zu machen.</t>
+  </si>
+  <si>
+    <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind mindestens 120s vorzuhalten und in dieser Zeit sind wiederholt Verbindungsversuche zu unternehmen.</t>
+  </si>
+  <si>
+    <t>Daten, die der Nachvollziehbarkeit dienen, sind, wenn möglich, gruppiert an externe Systeme zu senden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Metriken weiterzuleiten sind, soll bei Auftreten von bestimmten Metrikwerten oder Überschreitungen von Schwellen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Metriken weiterzuleiten sind, soll diese grafisch darstellen können.</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Fehler weiterzuleiten sind, soll bei Auftreten von bestimmten Fehlern oder Fehleranzahlen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Fehler weiterzuleiten sind, soll diese grafisch darstellen können.</t>
   </si>
 </sst>
 </file>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -687,7 +687,7 @@
     </row>
     <row r="3" spans="1:10" ht="45">
       <c r="B3" s="8" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -696,13 +696,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -716,13 +716,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -736,13 +736,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -773,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="J7" s="6"/>
     </row>
@@ -794,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -812,10 +812,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -833,10 +833,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -854,10 +854,10 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -875,10 +875,10 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="J12" s="6"/>
     </row>
@@ -896,10 +896,10 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="J13" s="6"/>
     </row>
@@ -917,14 +917,14 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="30">
+    <row r="15" spans="1:10">
       <c r="B15" s="8">
         <v>2130</v>
       </c>
@@ -938,10 +938,10 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -959,10 +959,10 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -980,10 +980,10 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -1001,10 +1001,10 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -1022,16 +1022,16 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="4"/>
@@ -1055,10 +1055,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J21" s="6"/>
     </row>
@@ -1076,10 +1076,10 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J22" s="6"/>
     </row>
@@ -1094,19 +1094,19 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="4"/>
@@ -1127,13 +1127,13 @@
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J25" s="6"/>
     </row>
@@ -1148,13 +1148,13 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J26" s="6"/>
     </row>
@@ -1163,19 +1163,19 @@
         <v>5021</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="J27" s="6"/>
     </row>
@@ -1190,13 +1190,13 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="J28" s="6"/>
     </row>
@@ -1211,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="J29" s="6"/>
     </row>
@@ -1232,13 +1232,13 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1247,19 +1247,19 @@
         <v>5040</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -1268,19 +1268,19 @@
         <v>5041</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1295,13 +1295,13 @@
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="J33" s="6"/>
     </row>
@@ -1316,13 +1316,13 @@
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="J34" s="6"/>
     </row>

</xml_diff>

<commit_message>
[ELAB-428] add some content to Anforderungen
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7ACA29-3067-4994-AFA2-F2690714C1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC884AD-F6B3-4E71-9356-93C498206C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="81">
   <si>
     <t>Id</t>
   </si>
@@ -191,18 +191,12 @@
     <t>Konzept</t>
   </si>
   <si>
-    <t>Demo-Anwendung</t>
-  </si>
-  <si>
     <t>Proof-of-Concept</t>
   </si>
   <si>
     <t>Anzahl Partnersysteme</t>
   </si>
   <si>
-    <t>Die Anzahl an zusätzlichen Partnersystemen, die für die Lösung benötigt werden, soll so gering wie möglich gehalten werden.</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -285,6 +279,24 @@
   </si>
   <si>
     <t>Das Partnersystem, zu dem die Fehler weiterzuleiten sind, soll diese grafisch darstellen können.</t>
+  </si>
+  <si>
+    <t>Structured Logging</t>
+  </si>
+  <si>
+    <t>Das Logging von Werten soll auf einem vordefinierten Format. Für ähnliche Funktionsgruppen (wie ein Schnittstellenaufruf) soll das gleiche Format verwendet werden. Ein anwendungsübergreifendes Format ist nicht gefordert.</t>
+  </si>
+  <si>
+    <t>Die Anzahl an zusätzlichen Partnersystemen, die für die Lösung benötigt werden, ist so gering zu halten wie möglich.</t>
+  </si>
+  <si>
+    <t>Bewertung Proof-of-Concept</t>
+  </si>
+  <si>
+    <t>Demoanwendung</t>
+  </si>
+  <si>
+    <t>Nach Abschluss der Implementierung des Proof-of-Concepts soll dieser veranschaulicht und bewertet werden. Grundlage hierfür sind diese Anforderungen sowie die, zu identifizierende, Fähigkeit die Fehlerszenarien der Demoanwendung nachvollziehbar zu gestalten.</t>
   </si>
 </sst>
 </file>
@@ -635,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -719,10 +731,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -739,110 +751,109 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60">
+      <c r="B6" s="8">
+        <v>1031</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="45">
-      <c r="B7" s="8">
-        <v>2010</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="45">
       <c r="B8" s="8">
+        <v>2010</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="45">
+      <c r="B9" s="8">
         <v>2011</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="60">
-      <c r="B9" s="8">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="60">
+      <c r="B10" s="8">
         <v>2020</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="45">
-      <c r="B10" s="8">
-        <v>2030</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="45">
       <c r="B11" s="8">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -854,16 +865,16 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="45">
       <c r="B12" s="8">
-        <v>2050</v>
+        <v>2040</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -875,58 +886,58 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="45">
       <c r="B13" s="8">
+        <v>2050</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="45">
+      <c r="B14" s="8">
         <v>2110</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="8">
-        <v>2120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="8">
-        <v>2130</v>
+        <v>2120</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -938,190 +949,199 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="30">
+    <row r="16" spans="1:10">
       <c r="B16" s="8">
+        <v>2130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="B17" s="8">
         <v>2140</v>
       </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="B17" s="8">
+      <c r="G17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="B18" s="8">
         <v>2150</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="B18" s="8">
+      <c r="G18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="8">
         <v>2160</v>
       </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="30">
+      <c r="B20" s="8">
+        <v>2161</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" ht="60">
+      <c r="B22" s="8">
+        <v>3010</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" ht="30">
-      <c r="B19" s="8">
-        <v>2161</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="45">
+      <c r="B23" s="8">
+        <v>3020</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" ht="60">
-      <c r="B21" s="8">
-        <v>3010</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" ht="45">
-      <c r="B22" s="8">
-        <v>3020</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="30">
-      <c r="B23" s="8">
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="30">
+      <c r="B24" s="8">
         <v>3100</v>
       </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="45">
+    <row r="25" spans="1:10" ht="60">
       <c r="B25" s="8">
-        <v>5010</v>
+        <v>3200</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1130,40 +1150,31 @@
         <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="45">
-      <c r="B26" s="8">
-        <v>5020</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>23</v>
-      </c>
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="45">
       <c r="B27" s="8">
-        <v>5021</v>
+        <v>5010</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1172,19 +1183,19 @@
         <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="45">
       <c r="B28" s="8">
-        <v>5022</v>
+        <v>5020</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1193,19 +1204,19 @@
         <v>22</v>
       </c>
       <c r="F28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="45">
+    <row r="29" spans="1:10" ht="30">
       <c r="B29" s="8">
-        <v>5030</v>
+        <v>5021</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1214,19 +1225,19 @@
         <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="30">
+    <row r="30" spans="1:10" ht="45">
       <c r="B30" s="8">
-        <v>5031</v>
+        <v>5022</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -1235,19 +1246,19 @@
         <v>22</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" ht="45">
       <c r="B31" s="8">
-        <v>5040</v>
+        <v>5030</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -1256,19 +1267,19 @@
         <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="30">
       <c r="B32" s="8">
-        <v>5041</v>
+        <v>5031</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -1277,19 +1288,19 @@
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="2:10" ht="45">
       <c r="B33" s="8">
-        <v>5042</v>
+        <v>5040</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1298,19 +1309,19 @@
         <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="2:10" ht="45">
+    <row r="34" spans="2:10" ht="30">
       <c r="B34" s="8">
-        <v>5050</v>
+        <v>5041</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1319,24 +1330,66 @@
         <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="2:10" ht="45">
+      <c r="B35" s="8">
+        <v>5042</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="2:10" ht="45">
+      <c r="B36" s="8">
+        <v>5050</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="G36" s="2"/>
+      <c r="J36" s="6"/>
     </row>
     <row r="37" spans="2:10">
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="2:10">
       <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="G40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[ELAB-432] corrected grammar issues, add missing paragraphs and polished a bit
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC884AD-F6B3-4E71-9356-93C498206C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEB1ABE-E9E4-405A-8A92-EB30AE029B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="1845" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     </r>
   </si>
   <si>
-    <t>Tritt ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, dass ein Nutzer einen neuen Datensatz angelegt möchte und wenn der diesen anlegt.</t>
-  </si>
-  <si>
     <t>Eigenschaften</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>Übertragung von Session-Replay-Daten</t>
   </si>
   <si>
-    <t>Es sollen Daten erhoben werden, anhand dessen die Benutzerinteraktionen und das Anwendungsverhalten nachgestellt werden kann. Diese Funktionalität darf jedoch standardmäßig deaktiviert sein.</t>
-  </si>
-  <si>
     <t>Datadump</t>
   </si>
   <si>
@@ -248,15 +242,9 @@
     <t>Sämtlich erfasste Session-Replay-Daten sind an ein Partnersystem weiterzuleiten.</t>
   </si>
   <si>
-    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so ist dieser automatisch zu erfasst und um weitere Attribute zu ergänzen.\par Sonstige Fehler können auch erfasst werden, aber hierbei Bedarf es einem manuellen Aufruf einer Schnittstelle</t>
-  </si>
-  <si>
     <t>Das Aufrufen von Schnittstellen ist mittels einer Logmeldung zu notieren. Hierbei sind relevante Informationen wie Aufrufparameter ebenfalls zu notieren.</t>
   </si>
   <si>
-    <t>Eine Demo-Anwendung ist zu Erstellen und soll dazu dienen, das Konzept darauf anwenden zu können.\par Diese Demo-Anwendung soll Fehlerverhalten beinhalten, die dann mithilfe der Lösung besser nachvollziehbar zu gestalten sind.</t>
-  </si>
-  <si>
     <t>Möglichkeit zum Export des fachlichen Modells des Frontends.</t>
   </si>
   <si>
@@ -284,9 +272,6 @@
     <t>Structured Logging</t>
   </si>
   <si>
-    <t>Das Logging von Werten soll auf einem vordefinierten Format. Für ähnliche Funktionsgruppen (wie ein Schnittstellenaufruf) soll das gleiche Format verwendet werden. Ein anwendungsübergreifendes Format ist nicht gefordert.</t>
-  </si>
-  <si>
     <t>Die Anzahl an zusätzlichen Partnersystemen, die für die Lösung benötigt werden, ist so gering zu halten wie möglich.</t>
   </si>
   <si>
@@ -297,6 +282,21 @@
   </si>
   <si>
     <t>Nach Abschluss der Implementierung des Proof-of-Concepts soll dieser veranschaulicht und bewertet werden. Grundlage hierfür sind diese Anforderungen sowie die, zu identifizierende, Fähigkeit die Fehlerszenarien der Demoanwendung nachvollziehbar zu gestalten.</t>
+  </si>
+  <si>
+    <t>Eine Demoanwendung ist zu Erstellen und soll dazu dienen, das Konzept darauf anwenden zu können.\par Diese Demoanwendung soll Fehlerverhalten beinhalten, die dann mithilfe der Lösung besser nachvollziehbar zu gestalten sind.</t>
+  </si>
+  <si>
+    <t>Tritt ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, wenn ein Nutzer ein Formular absendet.</t>
+  </si>
+  <si>
+    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so ist dieser automatisch zu erfasst und um weitere Attribute zu ergänzen.\par Sonstige Fehler können auch erfasst werden, aber hierbei ist keine automatische Erfassung gefordert.</t>
+  </si>
+  <si>
+    <t>Es sollen Session-Replay-Daten erhoben werden, anhand dessen die Benutzerinteraktionen und das Anwendungsverhalten nachgestellt werden kann. Diese Funktionalität darf jedoch standardmäßig deaktiviert sein.</t>
+  </si>
+  <si>
+    <t>Das Logging soll mit einem vordefinierten Format durchgeführt werden. Für ähnliche Funktionsgruppen (wie ein Schnittstellenaufruf) soll das gleiche Format verwendet werden. Ein anwendungsübergreifendes Format ist nicht gefordert.</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -699,22 +699,22 @@
     </row>
     <row r="3" spans="1:10" ht="45">
       <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -728,13 +728,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -748,13 +748,13 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60">
@@ -768,13 +768,13 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -805,11 +805,11 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="45">
+    <row r="9" spans="1:10" ht="30">
       <c r="B9" s="8">
         <v>2011</v>
       </c>
@@ -826,11 +826,11 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="60">
+    <row r="10" spans="1:10" ht="45">
       <c r="B10" s="8">
         <v>2020</v>
       </c>
@@ -844,10 +844,10 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -865,10 +865,10 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -886,10 +886,10 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="6"/>
     </row>
@@ -907,10 +907,10 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="J13" s="6"/>
     </row>
@@ -928,10 +928,10 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J14" s="6"/>
     </row>
@@ -949,10 +949,10 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -970,10 +970,10 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -991,10 +991,10 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -1012,10 +1012,10 @@
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -1033,10 +1033,10 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -1054,16 +1054,16 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="4"/>
@@ -1087,10 +1087,10 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J22" s="6"/>
     </row>
@@ -1108,10 +1108,10 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J23" s="6"/>
     </row>
@@ -1126,13 +1126,13 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J24" s="6"/>
     </row>
@@ -1141,25 +1141,25 @@
         <v>3200</v>
       </c>
       <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
         <v>21</v>
       </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>22</v>
-      </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
@@ -1180,13 +1180,13 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J27" s="6"/>
     </row>
@@ -1201,13 +1201,13 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J28" s="6"/>
     </row>
@@ -1216,19 +1216,19 @@
         <v>5021</v>
       </c>
       <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
         <v>21</v>
       </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J29" s="6"/>
     </row>
@@ -1243,13 +1243,13 @@
         <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1264,13 +1264,13 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -1285,13 +1285,13 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1300,19 +1300,19 @@
         <v>5040</v>
       </c>
       <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
         <v>21</v>
       </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J33" s="6"/>
     </row>
@@ -1321,19 +1321,19 @@
         <v>5041</v>
       </c>
       <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
         <v>21</v>
       </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>22</v>
-      </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J34" s="6"/>
     </row>
@@ -1348,13 +1348,13 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J35" s="6"/>
     </row>
@@ -1369,13 +1369,13 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J36" s="6"/>
     </row>

</xml_diff>

<commit_message>
[ELAB-432] WIP: incorporate feedback from cwa^2
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEB1ABE-E9E4-405A-8A92-EB30AE029B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C95FD9F-E97B-4CD5-88A7-B3CD84CEC330}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="1845" windowWidth="21600" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="1740" windowWidth="19410" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>1010</t>
   </si>
   <si>
-    <t>Es wird ein System konzipiert, welches darauf abzielt die Nachvollziehbarkeit eines Frontends zu verbessern. Speziell sollen Benutzerinteraktionen und Anwendungsverhalten nachvollziehbarer gemacht werden.</t>
-  </si>
-  <si>
     <t>Konzept</t>
   </si>
   <si>
@@ -245,12 +242,6 @@
     <t>Das Aufrufen von Schnittstellen ist mittels einer Logmeldung zu notieren. Hierbei sind relevante Informationen wie Aufrufparameter ebenfalls zu notieren.</t>
   </si>
   <si>
-    <t>Möglichkeit zum Export des fachlichen Modells des Frontends.</t>
-  </si>
-  <si>
-    <t>Re-Import des fachlichen Modells des Frontends, um diesen Zustand auf anderen Systemen und für andere Systeme einsehbar zu machen.</t>
-  </si>
-  <si>
     <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind mindestens 120s vorzuhalten und in dieser Zeit sind wiederholt Verbindungsversuche zu unternehmen.</t>
   </si>
   <si>
@@ -297,6 +288,15 @@
   </si>
   <si>
     <t>Das Logging soll mit einem vordefinierten Format durchgeführt werden. Für ähnliche Funktionsgruppen (wie ein Schnittstellenaufruf) soll das gleiche Format verwendet werden. Ein anwendungsübergreifendes Format ist nicht gefordert.</t>
+  </si>
+  <si>
+    <t>Es wird ein System konzipiert, welches darauf abzielt die Nachvollziehbarkeit einer JavaScript-basierten Webanwendung zu verbessern. Speziell sollen Benutzerinteraktionen und Anwendungsverhalten nachvollziehbarer gemacht werden.</t>
+  </si>
+  <si>
+    <t>Re-Import des fachlichen Modells der Webanwendung, um diesen Zustand auf anderen Systemen und für andere Systeme einsehbar zu machen.</t>
+  </si>
+  <si>
+    <t>Möglichkeit zum Export des fachlichen Modells der Webanwendung.</t>
   </si>
 </sst>
 </file>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -697,7 +697,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="60">
       <c r="B3" s="8" t="s">
         <v>40</v>
       </c>
@@ -711,10 +711,10 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -731,10 +731,10 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -751,10 +751,10 @@
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60">
@@ -771,10 +771,10 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -805,7 +805,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -826,7 +826,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -847,7 +847,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -910,7 +910,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J13" s="6"/>
     </row>
@@ -931,7 +931,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J14" s="6"/>
     </row>
@@ -952,7 +952,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -973,7 +973,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -994,7 +994,7 @@
         <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -1015,7 +1015,7 @@
         <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="6"/>
     </row>
@@ -1036,7 +1036,7 @@
         <v>38</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -1057,7 +1057,7 @@
         <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="J20" s="6"/>
     </row>
@@ -1090,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J22" s="6"/>
     </row>
@@ -1111,7 +1111,7 @@
         <v>16</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J23" s="6"/>
     </row>
@@ -1126,13 +1126,13 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J24" s="6"/>
     </row>
@@ -1150,10 +1150,10 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J25" s="6"/>
     </row>
@@ -1183,7 +1183,7 @@
         <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>19</v>
@@ -1204,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>22</v>
@@ -1225,10 +1225,10 @@
         <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J29" s="6"/>
     </row>
@@ -1246,10 +1246,10 @@
         <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1267,7 +1267,7 @@
         <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>24</v>
@@ -1288,7 +1288,7 @@
         <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>25</v>
@@ -1309,7 +1309,7 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>23</v>
@@ -1330,10 +1330,10 @@
         <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J34" s="6"/>
     </row>
@@ -1351,10 +1351,10 @@
         <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J35" s="6"/>
     </row>
@@ -1372,7 +1372,7 @@
         <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
[ELAB-432] incorporate feedback by prof
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C95FD9F-E97B-4CD5-88A7-B3CD84CEC330}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C7CF54-1DA9-4525-A045-47EFA618C190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="1740" windowWidth="19410" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="19410" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
   <si>
     <t>Id</t>
   </si>
@@ -170,12 +170,6 @@
     <t>Übertragung von Session-Replay-Daten</t>
   </si>
   <si>
-    <t>Datadump</t>
-  </si>
-  <si>
-    <t>Datadump-Import</t>
-  </si>
-  <si>
     <t>1010</t>
   </si>
   <si>
@@ -293,10 +287,7 @@
     <t>Es wird ein System konzipiert, welches darauf abzielt die Nachvollziehbarkeit einer JavaScript-basierten Webanwendung zu verbessern. Speziell sollen Benutzerinteraktionen und Anwendungsverhalten nachvollziehbarer gemacht werden.</t>
   </si>
   <si>
-    <t>Re-Import des fachlichen Modells der Webanwendung, um diesen Zustand auf anderen Systemen und für andere Systeme einsehbar zu machen.</t>
-  </si>
-  <si>
-    <t>Möglichkeit zum Export des fachlichen Modells der Webanwendung.</t>
+    <t>nf</t>
   </si>
 </sst>
 </file>
@@ -647,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -699,7 +690,7 @@
     </row>
     <row r="3" spans="1:10" ht="60">
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -711,10 +702,10 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60">
@@ -731,10 +722,10 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -751,10 +742,10 @@
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60">
@@ -771,10 +762,10 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -805,7 +796,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -826,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -847,7 +838,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" s="6"/>
     </row>
@@ -910,7 +901,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J13" s="6"/>
     </row>
@@ -931,7 +922,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J14" s="6"/>
     </row>
@@ -952,7 +943,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -973,7 +964,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -994,7 +985,7 @@
         <v>36</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -1015,133 +1006,124 @@
         <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="60">
+      <c r="B20" s="8">
+        <v>3010</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="B19" s="8">
-        <v>2160</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="30">
-      <c r="B20" s="8">
-        <v>2161</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+    <row r="21" spans="1:10" ht="45">
+      <c r="B21" s="8">
+        <v>3020</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="60">
+    <row r="22" spans="1:10" ht="30">
       <c r="B22" s="8">
-        <v>3010</v>
+        <v>3100</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="45">
+    <row r="23" spans="1:10" ht="60">
       <c r="B23" s="8">
-        <v>3020</v>
+        <v>3200</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="30">
-      <c r="B24" s="8">
-        <v>3100</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>69</v>
-      </c>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="60">
+    <row r="25" spans="1:10" ht="45">
       <c r="B25" s="8">
-        <v>3200</v>
+        <v>5010</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -1150,31 +1132,40 @@
         <v>21</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+    <row r="26" spans="1:10" ht="45">
+      <c r="B26" s="8">
+        <v>5020</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="45">
+    <row r="27" spans="1:10" ht="30">
       <c r="B27" s="8">
-        <v>5010</v>
+        <v>5021</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1186,16 +1177,16 @@
         <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="45">
       <c r="B28" s="8">
-        <v>5020</v>
+        <v>5022</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1207,16 +1198,16 @@
         <v>46</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="30">
+    <row r="29" spans="1:10" ht="45">
       <c r="B29" s="8">
-        <v>5021</v>
+        <v>5030</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1228,16 +1219,16 @@
         <v>47</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="45">
+    <row r="30" spans="1:10" ht="30">
       <c r="B30" s="8">
-        <v>5022</v>
+        <v>5031</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -1249,16 +1240,16 @@
         <v>48</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" ht="45">
       <c r="B31" s="8">
-        <v>5030</v>
+        <v>5040</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -1270,16 +1261,16 @@
         <v>49</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="30">
       <c r="B32" s="8">
-        <v>5031</v>
+        <v>5041</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
@@ -1291,16 +1282,16 @@
         <v>50</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="2:10" ht="45">
       <c r="B33" s="8">
-        <v>5040</v>
+        <v>5042</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1312,16 +1303,16 @@
         <v>51</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="2:10" ht="30">
+    <row r="34" spans="2:10" ht="45">
       <c r="B34" s="8">
-        <v>5041</v>
+        <v>5050</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1333,63 +1324,21 @@
         <v>52</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="2:10" ht="45">
-      <c r="B35" s="8">
-        <v>5042</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="2:10" ht="45">
-      <c r="B36" s="8">
-        <v>5050</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J36" s="6"/>
+    <row r="35" spans="2:10">
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="2:10">
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="2:10">
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="G40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[ELAB-428] adapt feedback from prof for 'Anforderungen'
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C7CF54-1DA9-4525-A045-47EFA618C190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541FE1A8-CC53-4E60-82EB-1232363F451D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="19410" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Gruppe</t>
   </si>
   <si>
-    <t>Grundanforderungen</t>
-  </si>
-  <si>
     <t>Funktionsumfang</t>
   </si>
   <si>
@@ -61,12 +58,6 @@
   </si>
   <si>
     <t>Beschreibung</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>f</t>
   </si>
   <si>
     <t>S</t>
@@ -113,27 +104,9 @@
     <t>A</t>
   </si>
   <si>
-    <t>Es existiert ein Partnersystem, zu dem Logmeldungen weitergeleitet werden. Dieses System soll die Logmeldungen speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Logmeldungen bieten.</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>A+S</t>
   </si>
   <si>
-    <t>Es existiert ein Partnersystem, zu dem Fehler weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Fehler bieten.</t>
-  </si>
-  <si>
-    <t>Es existiert ein Partnersystem, zu dem Metriken weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Metriken bieten.</t>
-  </si>
-  <si>
-    <t>Es existiert ein Partnersystem, zu dem Tracingdaten weitergeleitet werden. Dieses System soll die Fehler speichern und den Entwicklern und Betreibern eine Einsicht in die erfassten Tracingdaten bieten.</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Tracingdaten weitergeleitet werden, soll diese grafisch als Tracing-Wasserfallgraph darstellen können.</t>
-  </si>
-  <si>
     <t>Error-Monitoring</t>
   </si>
   <si>
@@ -143,15 +116,6 @@
     <t>Metriken</t>
   </si>
   <si>
-    <t>Es werden Tracingdaten ähnlich wie bei OpenTracing und OpenTelemetry erfasst.\par Optimalerweise werden die Tracingdaten mit OpenTelemetry-konformen Komponenten erfasst.</t>
-  </si>
-  <si>
-    <t>Es werden Metrikdaten ähnlich wie bei OpenTelemetry erfasst.\par Optimalerweise werden die Tracingdaten mit OpenTelemetry-konformen Komponenten erfasst.</t>
-  </si>
-  <si>
-    <t>Es existiert ein Partnersystem, zu die Session-Replay-Daten weitergeleitet werden. Dieses System soll anhand dieser Daten eine Benutzersitzung rekreieren können.</t>
-  </si>
-  <si>
     <t>Session-Replay</t>
   </si>
   <si>
@@ -170,15 +134,6 @@
     <t>Übertragung von Session-Replay-Daten</t>
   </si>
   <si>
-    <t>1010</t>
-  </si>
-  <si>
-    <t>Konzept</t>
-  </si>
-  <si>
-    <t>Proof-of-Concept</t>
-  </si>
-  <si>
     <t>Anzahl Partnersysteme</t>
   </si>
   <si>
@@ -215,79 +170,142 @@
     <t>Partnersystem \textit{Session-Replay}</t>
   </si>
   <si>
-    <t>Auf Basis des Konzeptes, ist die Demo-Anwendung zu erweitern.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Tracingdaten sind an ein Partnersystem weiterzuleiten.</t>
-  </si>
-  <si>
-    <t>Ausgewählte Logmeldungen sind an ein Partnersystem weiterzuleiten. Die Auswahl könnte über die Kritikalität, also dem Log-Level, der Logmeldung erfolgen.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Fehler sind an ein Partnersystem weiterzuleiten.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Metrikdaten sind an ein Partnersystem weiterzuleiten.</t>
-  </si>
-  <si>
-    <t>Sämtlich erfasste Session-Replay-Daten sind an ein Partnersystem weiterzuleiten.</t>
-  </si>
-  <si>
-    <t>Das Aufrufen von Schnittstellen ist mittels einer Logmeldung zu notieren. Hierbei sind relevante Informationen wie Aufrufparameter ebenfalls zu notieren.</t>
-  </si>
-  <si>
     <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind mindestens 120s vorzuhalten und in dieser Zeit sind wiederholt Verbindungsversuche zu unternehmen.</t>
   </si>
   <si>
     <t>Daten, die der Nachvollziehbarkeit dienen, sind, wenn möglich, gruppiert an externe Systeme zu senden. Hierbei ist eine kurze Aggregationszeit von bis zu 10s akzeptabel.</t>
   </si>
   <si>
-    <t>Das Partnersystem, zu dem die Metriken weiterzuleiten sind, soll bei Auftreten von bestimmten Metrikwerten oder Überschreitungen von Schwellen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Metriken weiterzuleiten sind, soll diese grafisch darstellen können.</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Fehler weiterzuleiten sind, soll bei Auftreten von bestimmten Fehlern oder Fehleranzahlen eine Meldung erzeugen (per E-Mail, Slack, o. Ä.).</t>
-  </si>
-  <si>
-    <t>Das Partnersystem, zu dem die Fehler weiterzuleiten sind, soll diese grafisch darstellen können.</t>
-  </si>
-  <si>
     <t>Structured Logging</t>
   </si>
   <si>
     <t>Die Anzahl an zusätzlichen Partnersystemen, die für die Lösung benötigt werden, ist so gering zu halten wie möglich.</t>
   </si>
   <si>
-    <t>Bewertung Proof-of-Concept</t>
-  </si>
-  <si>
-    <t>Demoanwendung</t>
-  </si>
-  <si>
-    <t>Nach Abschluss der Implementierung des Proof-of-Concepts soll dieser veranschaulicht und bewertet werden. Grundlage hierfür sind diese Anforderungen sowie die, zu identifizierende, Fähigkeit die Fehlerszenarien der Demoanwendung nachvollziehbar zu gestalten.</t>
-  </si>
-  <si>
-    <t>Eine Demoanwendung ist zu Erstellen und soll dazu dienen, das Konzept darauf anwenden zu können.\par Diese Demoanwendung soll Fehlerverhalten beinhalten, die dann mithilfe der Lösung besser nachvollziehbar zu gestalten sind.</t>
-  </si>
-  <si>
-    <t>Tritt ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, wenn ein Nutzer ein Formular absendet.</t>
-  </si>
-  <si>
-    <t>Tritt ein Fehler auf, der nicht gefangen wurde, so ist dieser automatisch zu erfasst und um weitere Attribute zu ergänzen.\par Sonstige Fehler können auch erfasst werden, aber hierbei ist keine automatische Erfassung gefordert.</t>
-  </si>
-  <si>
-    <t>Es sollen Session-Replay-Daten erhoben werden, anhand dessen die Benutzerinteraktionen und das Anwendungsverhalten nachgestellt werden kann. Diese Funktionalität darf jedoch standardmäßig deaktiviert sein.</t>
-  </si>
-  <si>
     <t>Das Logging soll mit einem vordefinierten Format durchgeführt werden. Für ähnliche Funktionsgruppen (wie ein Schnittstellenaufruf) soll das gleiche Format verwendet werden. Ein anwendungsübergreifendes Format ist nicht gefordert.</t>
   </si>
   <si>
-    <t>Es wird ein System konzipiert, welches darauf abzielt die Nachvollziehbarkeit einer JavaScript-basierten Webanwendung zu verbessern. Speziell sollen Benutzerinteraktionen und Anwendungsverhalten nachvollziehbarer gemacht werden.</t>
-  </si>
-  <si>
-    <t>nf</t>
+    <t>Wird ein nicht abgefangener Fehler im JavaScript-Kontext geworfen, so ist dieser automatisch zu erfassen und um weitere Attribute zu ergänzen.\par Abgefangene und behandelte Fehler können ebenso erfasst werden, jedoch ist hierbei keine automatische Erfassung gefordert.</t>
+  </si>
+  <si>
+    <t>Im Frontend sowie im Backend sind Tracing Spans zu erstellen, die Business-Methoden sowie Schnittstellenaufrufe umschließen. Bei einem Schnittstellaufruf sind die Informationen des Spankontextes über einen Traceheader zu übergeben, sodass die subsequent erstellten Spans hiermit assoziiert werden können.</t>
+  </si>
+  <si>
+    <t>Tracing-Standard</t>
+  </si>
+  <si>
+    <t>Das Tracing soll einem gängigen Standard (wie OpenTelemetry oder OpenTracing) folgen.</t>
+  </si>
+  <si>
+    <t>Metrik-Standard</t>
+  </si>
+  <si>
+    <t>Metriken sollen nach einem gängigen Standard (wie OpenTelemetry) erfasst werden.</t>
+  </si>
+  <si>
+    <t>vielleicht erweitern?</t>
+  </si>
+  <si>
+    <t>Im Frontend sind beispielhaft Metriken zu erheben, wie z. B. die Zeit bis der Nutzer interagieren kann (Time to Interactive (TTI)) oder die Anzahl an Aufrufen je Schnittstelle</t>
+  </si>
+  <si>
+    <t>Schalter für Session-Replay</t>
+  </si>
+  <si>
+    <t>Beim ersten Aufruf des Frontends sind keine Session-Replay-Daten zu erheben.\par Stattdessen soll der Nutzer über einen Dialog auswählen können, ob er der Aufnahme zustimmt und erst danach sind diese Daten zu erheben.</t>
+  </si>
+  <si>
+    <t>Im Frontend sind Daten zwecks Session-Replay zu erheben, welche u. A. Benutzerinteraktionen, Schnittstellaufrufe sowie DOM-Manipulationen enthalten.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Fehler des Frontends sind an ein "Error-Monitoring"-Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Im Frontend ist das Aufrufen von Schnittstellen ist mittels einer Logmeldung zu notieren. Hierbei soll vor Aufruf geloggt werden, welche Schnittstelle aufgerufen wird und mit welchen Parametern. Nach dem Aufruf soll bei Erfolg das Ergebnisobjekt geloggt werden, und bei einem Fehler soll dieser notiert werden.</t>
+  </si>
+  <si>
+    <t>Tritt im Frontend ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, wenn ein Nutzer das Absenden eines Formular initiiert.</t>
+  </si>
+  <si>
+    <t>Logmeldungen des Frontends sind an ein "Log-Management"-Partnersystem weiterzuleiten.\par Dabei sind Logmeldungen ab dem Log-Level "DEBUG" und höher zu übertragen.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Tracingdaten von Front- und Backend sind an ein "Tracing"-Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Sämtlich erfasste Metriken des Frontends sind an ein "Metrik"-Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Sämtlich im Frontend erfasste Daten zum Session-Replay sind an ein "Session-Replay"-Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Das Partnersystem, zu dem die Tracingdaten weitergeleitet werden, soll diese grafisch als Trace-Gantt-Diagramm darstellen können.</t>
+  </si>
+  <si>
+    <t>Manuelle Analyse \textit{Log-Management}</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Log-Management"-Partnersystem, zu dem Logmeldungen weitergeleitet werden und welches diese speichert.</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Error-Monitoring"-Partnersystem, zu dem Fehler weitergeleitet werden und welches diese persistiert.</t>
+  </si>
+  <si>
+    <t>Die Fehler sollen bspw. in Histogrammen grafisch dargestellt werden können.</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Tracing"-Partnersystem, welches die Tracingdaten konsumiert und speichert. Zusammengehörige Spans sind zu Traces zusammenzufassen.</t>
+  </si>
+  <si>
+    <t>Die erfassten Tracingdaten sind für die Nutzer des Systems einsehbar, sowie können diese gefiltert werden. Die Filtierung erfolgt auf Basis von Eigenschaften der Tracingdaten (wie Name des meldenden Systems).</t>
+  </si>
+  <si>
+    <t>Nutzer des Systems sollen die erfassten Fehler einsehen sowie diese filtern können. Die Filtierung erfolgt auf Basis der Eigenschaften der Fehler (bspw. der Fehlername).</t>
+  </si>
+  <si>
+    <t>Nutzer des Systems sollen die erfassten Logmeldungen einsehen sowie diese filtern können. Die Filtierung erfolgt auf Basis der Eigenschaften der Logmeldung (bspw. des Log-Levels).</t>
+  </si>
+  <si>
+    <t>Metriken sind grafisch darstellbar, bspw. in Histogrammen.</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Metrik"-Partnersystem, zu dem Metriken weitergeleitet werden und welches diese persistiert.</t>
+  </si>
+  <si>
+    <t>Bei Auftreten von bestimmten Metrikwerten oder Überschreitungen von Schwellen soll eine Meldung erzeugt werden können (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Bei Auftreten von bestimmten Fehlern oder einer Anzahl von Fehlern soll eine Meldung erzeugt werden können (per E-Mail, Slack, o. Ä.).</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Session-Replay"-Partnersystem, zu die Daten zum Session-Replay gesendet werden und welches diese analysiert und speichert.</t>
+  </si>
+  <si>
+    <t>Dieses System soll anhand der Daten jede aufgezeichnete Benutzersitzung in Videoform nachstellen.</t>
+  </si>
+  <si>
+    <t>Nachstellung \textit{Session-Replay}</t>
+  </si>
+  <si>
+    <t>Basis.</t>
+  </si>
+  <si>
+    <t>Leistungs.</t>
+  </si>
+  <si>
+    <t>Begeist.</t>
+  </si>
+  <si>
+    <t>f.</t>
+  </si>
+  <si>
+    <t>n. f.</t>
+  </si>
+  <si>
+    <t>Manuelle Analyse \textit{Error-Monitoring}</t>
+  </si>
+  <si>
+    <t>Manuelle Analyse \textit{Tracing}</t>
   </si>
 </sst>
 </file>
@@ -638,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -651,7 +669,7 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.42578125" customWidth="1"/>
+    <col min="7" max="7" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -671,10 +689,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -689,656 +707,712 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="60">
-      <c r="B3" s="8" t="s">
-        <v>38</v>
+      <c r="B3" s="8">
+        <v>2110</v>
       </c>
       <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="45">
+      <c r="B4" s="8">
+        <v>2111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="60">
-      <c r="B4" s="8">
-        <v>1020</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>56</v>
+      </c>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="45">
       <c r="B5" s="8">
-        <v>1030</v>
+        <v>2120</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="60">
       <c r="B6" s="8">
-        <v>1031</v>
+        <v>2210</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="B7" s="8">
+        <v>2220</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="60">
+      <c r="B8" s="8">
+        <v>2310</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="45">
-      <c r="B8" s="8">
-        <v>2010</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="30">
       <c r="B9" s="8">
-        <v>2011</v>
+        <v>2311</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="30">
       <c r="B10" s="8">
-        <v>2020</v>
+        <v>2320</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="45">
       <c r="B11" s="8">
-        <v>2030</v>
+        <v>2410</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="30">
+      <c r="B12" s="8">
+        <v>2411</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="B13" s="8">
+        <v>2420</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="30">
+      <c r="B14" s="8">
+        <v>2510</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="45">
+      <c r="B15" s="8">
+        <v>2511</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="30">
+      <c r="B16" s="8">
+        <v>2520</v>
+      </c>
+      <c r="C16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="60">
+      <c r="B18" s="8">
+        <v>3010</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="45">
+      <c r="B19" s="8">
+        <v>3020</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="30">
+      <c r="B20" s="8">
+        <v>3100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="45">
-      <c r="B12" s="8">
-        <v>2040</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="45">
-      <c r="B13" s="8">
-        <v>2050</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" ht="45">
-      <c r="B14" s="8">
-        <v>2110</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="8">
-        <v>2120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="8">
-        <v>2130</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="B17" s="8">
-        <v>2140</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="B18" s="8">
-        <v>2150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="60">
-      <c r="B20" s="8">
-        <v>3010</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="45">
       <c r="B21" s="8">
-        <v>3020</v>
+        <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="30">
+      <c r="B23" s="8">
+        <v>5100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" ht="30">
-      <c r="B22" s="8">
-        <v>3100</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="60">
-      <c r="B23" s="8">
-        <v>3200</v>
-      </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+    <row r="24" spans="1:10" ht="45">
+      <c r="B24" s="8">
+        <v>5110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="45">
+    <row r="25" spans="1:10" ht="30">
       <c r="B25" s="8">
-        <v>5010</v>
+        <v>5200</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="45">
       <c r="B26" s="8">
-        <v>5020</v>
+        <v>5210</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10">
       <c r="B27" s="8">
-        <v>5021</v>
+        <v>5220</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>65</v>
       </c>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="45">
+    <row r="28" spans="1:10" ht="30">
       <c r="B28" s="8">
-        <v>5022</v>
+        <v>5230</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="45">
+    <row r="29" spans="1:10" ht="30">
       <c r="B29" s="8">
-        <v>5030</v>
+        <v>5300</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="30">
+    <row r="30" spans="1:10" ht="45">
       <c r="B30" s="8">
-        <v>5031</v>
+        <v>5310</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="45">
+    <row r="31" spans="1:10" ht="30">
       <c r="B31" s="8">
-        <v>5040</v>
+        <v>5320</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="30">
       <c r="B32" s="8">
-        <v>5041</v>
+        <v>5400</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="2:10" ht="45">
+    <row r="33" spans="2:10">
       <c r="B33" s="8">
-        <v>5042</v>
+        <v>5410</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="2:10" ht="45">
+    <row r="34" spans="2:10" ht="30">
       <c r="B34" s="8">
-        <v>5050</v>
+        <v>5420</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="2:10">
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="G36" s="2"/>
+    <row r="35" spans="2:10" ht="30">
+      <c r="B35" s="8">
+        <v>5500</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="2:10" ht="30">
+      <c r="B36" s="8">
+        <v>5510</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="6"/>
     </row>
     <row r="37" spans="2:10">
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="2:10">
       <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="G39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[ELAB-430] reword of 'Konzept'
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79976C0-EC27-4989-BFCA-E3C3757EA43B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2429CF6D-AAA5-4EAE-975F-E185F41C659C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>Id</t>
   </si>
@@ -203,12 +203,6 @@
     <t>Metriken sollen nach einem gängigen Standard (wie OpenTelemetry) erfasst werden.</t>
   </si>
   <si>
-    <t>vielleicht erweitern?</t>
-  </si>
-  <si>
-    <t>Im Frontend sind beispielhaft Metriken zu erheben, wie z. B. die Zeit bis der Nutzer interagieren kann (Time to Interactive (TTI)) oder die Anzahl an Aufrufen je Schnittstelle</t>
-  </si>
-  <si>
     <t>Schalter für Session-Replay</t>
   </si>
   <si>
@@ -306,6 +300,21 @@
   </si>
   <si>
     <t>Manuelle Analyse \textit{Tracing}</t>
+  </si>
+  <si>
+    <t>Im Frontend sind beispielhaft Metriken zu erheben, wie z. B. die Anzahl an Produkten oder die Anzahl an aufgetretenen</t>
+  </si>
+  <si>
+    <t>Erfüllunggrad</t>
+  </si>
+  <si>
+    <t>TODO: check</t>
+  </si>
+  <si>
+    <t>TODO: zeigen</t>
+  </si>
+  <si>
+    <t>TODO: einbauen?</t>
   </si>
 </sst>
 </file>
@@ -358,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,6 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -658,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -670,6 +680,8 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="74.85546875" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -693,6 +705,9 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -705,16 +720,17 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="60">
       <c r="B3" s="8">
         <v>2110</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -723,7 +739,10 @@
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
       </c>
       <c r="J3" s="6"/>
     </row>
@@ -732,10 +751,10 @@
         <v>2111</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -744,7 +763,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="I4" s="9">
+        <v>1</v>
       </c>
       <c r="J4" s="6"/>
     </row>
@@ -753,10 +775,10 @@
         <v>2120</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -765,7 +787,10 @@
         <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
       </c>
       <c r="J5" s="6"/>
     </row>
@@ -774,10 +799,10 @@
         <v>2210</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -787,6 +812,9 @@
       </c>
       <c r="G6" s="2" t="s">
         <v>43</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1</v>
       </c>
       <c r="J6" s="6"/>
     </row>
@@ -795,10 +823,10 @@
         <v>2220</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -807,7 +835,10 @@
         <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
       </c>
       <c r="J7" s="6"/>
     </row>
@@ -816,10 +847,10 @@
         <v>2310</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -829,6 +860,9 @@
       </c>
       <c r="G8" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -837,10 +871,10 @@
         <v>2311</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -850,6 +884,9 @@
       </c>
       <c r="G9" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
       </c>
       <c r="J9" s="6"/>
     </row>
@@ -858,10 +895,10 @@
         <v>2320</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -870,19 +907,22 @@
         <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
       </c>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="30">
       <c r="B11" s="8">
         <v>2410</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -891,10 +931,10 @@
         <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" t="s">
-        <v>49</v>
+        <v>82</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1</v>
       </c>
       <c r="J11" s="6"/>
     </row>
@@ -903,10 +943,10 @@
         <v>2411</v>
       </c>
       <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
         <v>79</v>
-      </c>
-      <c r="D12" t="s">
-        <v>81</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -916,6 +956,9 @@
       </c>
       <c r="G12" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
       </c>
       <c r="J12" s="6"/>
     </row>
@@ -924,10 +967,10 @@
         <v>2420</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -936,19 +979,22 @@
         <v>24</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1</v>
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="30">
+    <row r="14" spans="1:10" ht="45">
       <c r="B14" s="8">
         <v>2510</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -957,7 +1003,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="I14" s="9">
+        <v>1</v>
       </c>
       <c r="J14" s="6"/>
     </row>
@@ -966,19 +1015,22 @@
         <v>2511</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1</v>
       </c>
       <c r="J15" s="6"/>
     </row>
@@ -987,10 +1039,10 @@
         <v>2520</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -999,7 +1051,10 @@
         <v>25</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -1020,10 +1075,10 @@
         <v>3010</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1034,17 +1089,19 @@
       <c r="G18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="45">
       <c r="B19" s="8">
         <v>3020</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1055,17 +1112,22 @@
       <c r="G19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="30">
       <c r="B20" s="8">
         <v>3100</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -1075,6 +1137,9 @@
       </c>
       <c r="G20" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.7</v>
       </c>
       <c r="J20" s="6"/>
     </row>
@@ -1083,10 +1148,10 @@
         <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1097,7 +1162,9 @@
       <c r="G21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
@@ -1116,10 +1183,10 @@
         <v>5100</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1128,7 +1195,10 @@
         <v>28</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1</v>
       </c>
       <c r="J23" s="6"/>
     </row>
@@ -1137,19 +1207,22 @@
         <v>5110</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1</v>
       </c>
       <c r="J24" s="6"/>
     </row>
@@ -1158,10 +1231,10 @@
         <v>5200</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1170,7 +1243,10 @@
         <v>29</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1</v>
       </c>
       <c r="J25" s="6"/>
     </row>
@@ -1179,19 +1255,22 @@
         <v>5210</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1</v>
       </c>
       <c r="J26" s="6"/>
     </row>
@@ -1200,10 +1279,10 @@
         <v>5220</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -1212,7 +1291,10 @@
         <v>30</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
       </c>
       <c r="J27" s="6"/>
     </row>
@@ -1221,10 +1303,10 @@
         <v>5230</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -1233,19 +1315,24 @@
         <v>31</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J28" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="30">
       <c r="B29" s="8">
         <v>5300</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
@@ -1254,7 +1341,10 @@
         <v>32</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="I29" s="9">
+        <v>1</v>
       </c>
       <c r="J29" s="6"/>
     </row>
@@ -1263,19 +1353,22 @@
         <v>5310</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1</v>
       </c>
       <c r="J30" s="6"/>
     </row>
@@ -1284,10 +1377,10 @@
         <v>5320</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
@@ -1296,7 +1389,10 @@
         <v>33</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="I31" s="9">
+        <v>1</v>
       </c>
       <c r="J31" s="6"/>
     </row>
@@ -1305,10 +1401,10 @@
         <v>5400</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
@@ -1317,7 +1413,10 @@
         <v>34</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1</v>
       </c>
       <c r="J32" s="6"/>
     </row>
@@ -1326,10 +1425,10 @@
         <v>5410</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
@@ -1338,7 +1437,10 @@
         <v>35</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="I33" s="9">
+        <v>1</v>
       </c>
       <c r="J33" s="6"/>
     </row>
@@ -1347,10 +1449,10 @@
         <v>5420</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
         <v>16</v>
@@ -1359,19 +1461,24 @@
         <v>36</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J34" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="35" spans="2:10" ht="30">
       <c r="B35" s="8">
         <v>5500</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -1380,7 +1487,10 @@
         <v>37</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1</v>
       </c>
       <c r="J35" s="6"/>
     </row>
@@ -1389,19 +1499,22 @@
         <v>5510</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="I36" s="9">
+        <v>1</v>
       </c>
       <c r="J36" s="6"/>
     </row>

</xml_diff>

<commit_message>
[ELAB-437] added script to convert Anforderungsliste.xlsx to rated table
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2429CF6D-AAA5-4EAE-975F-E185F41C659C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12614434-FAF1-4D66-9D74-39CFD75D66BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="600" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Im Frontend sind beispielhaft Metriken zu erheben, wie z. B. die Anzahl an Produkten oder die Anzahl an aufgetretenen</t>
   </si>
   <si>
-    <t>Erfüllunggrad</t>
-  </si>
-  <si>
     <t>TODO: check</t>
   </si>
   <si>
@@ -315,6 +312,18 @@
   </si>
   <si>
     <t>TODO: einbauen?</t>
+  </si>
+  <si>
+    <t>Erf{\"u}llungsgrad</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>70%</t>
   </si>
 </sst>
 </file>
@@ -367,9 +376,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -379,13 +387,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -668,14 +680,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
@@ -685,393 +698,407 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>83</v>
+      <c r="I1" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="60">
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>2110</v>
       </c>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="9">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="45">
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>2111</v>
       </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="45">
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>2120</v>
       </c>
-      <c r="C5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="9">
-        <v>1</v>
-      </c>
-      <c r="J5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="60">
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>2210</v>
       </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="9">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="30">
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>2220</v>
       </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="9">
-        <v>1</v>
-      </c>
-      <c r="J7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" ht="60">
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>2310</v>
       </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="9">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="30">
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>2311</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>2320</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="9">
-        <v>1</v>
-      </c>
-      <c r="J10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>2410</v>
       </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="9">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>2411</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="9">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>2420</v>
       </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I13" s="9">
-        <v>1</v>
-      </c>
-      <c r="J13" s="6"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="45">
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>2510</v>
       </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="9">
-        <v>1</v>
-      </c>
-      <c r="J14" s="6"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="45">
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>2511</v>
       </c>
-      <c r="C15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="9">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30">
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>2520</v>
       </c>
-      <c r="C16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="9">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="J17" s="6"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="60">
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>3010</v>
       </c>
       <c r="C18" t="s">
@@ -1086,15 +1113,15 @@
       <c r="F18" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>84</v>
+      <c r="J18" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="45">
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>3020</v>
       </c>
       <c r="C19" t="s">
@@ -1109,18 +1136,18 @@
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="9">
-        <v>1</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>85</v>
+      <c r="I19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>3100</v>
       </c>
       <c r="C20" t="s">
@@ -1135,16 +1162,16 @@
       <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="J20" s="6"/>
+      <c r="I20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="45">
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>3200</v>
       </c>
       <c r="C21" t="s">
@@ -1159,27 +1186,27 @@
       <c r="F21" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>84</v>
+      <c r="J21" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="J22" s="6"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" ht="30">
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>5100</v>
       </c>
       <c r="C23" t="s">
@@ -1194,16 +1221,16 @@
       <c r="F23" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I23" s="9">
-        <v>1</v>
-      </c>
-      <c r="J23" s="6"/>
+      <c r="I23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" ht="45">
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>5110</v>
       </c>
       <c r="C24" t="s">
@@ -1218,16 +1245,16 @@
       <c r="F24" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="9">
-        <v>1</v>
-      </c>
-      <c r="J24" s="6"/>
+      <c r="I24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <v>5200</v>
       </c>
       <c r="C25" t="s">
@@ -1242,16 +1269,16 @@
       <c r="F25" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="9">
-        <v>1</v>
-      </c>
-      <c r="J25" s="6"/>
+      <c r="I25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="45">
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <v>5210</v>
       </c>
       <c r="C26" t="s">
@@ -1266,16 +1293,16 @@
       <c r="F26" t="s">
         <v>80</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I26" s="9">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6"/>
+      <c r="I26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>5220</v>
       </c>
       <c r="C27" t="s">
@@ -1290,16 +1317,16 @@
       <c r="F27" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I27" s="9">
-        <v>1</v>
-      </c>
-      <c r="J27" s="6"/>
+      <c r="I27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="30">
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>5230</v>
       </c>
       <c r="C28" t="s">
@@ -1314,18 +1341,18 @@
       <c r="F28" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I28" s="9">
-        <v>0</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>86</v>
+      <c r="I28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
-      <c r="B29" s="8">
+      <c r="B29" s="6">
         <v>5300</v>
       </c>
       <c r="C29" t="s">
@@ -1340,16 +1367,16 @@
       <c r="F29" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I29" s="9">
-        <v>1</v>
-      </c>
-      <c r="J29" s="6"/>
+      <c r="I29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" ht="45">
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>5310</v>
       </c>
       <c r="C30" t="s">
@@ -1364,16 +1391,16 @@
       <c r="F30" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I30" s="9">
-        <v>1</v>
-      </c>
-      <c r="J30" s="6"/>
+      <c r="I30" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="B31" s="8">
+      <c r="B31" s="6">
         <v>5320</v>
       </c>
       <c r="C31" t="s">
@@ -1388,16 +1415,16 @@
       <c r="F31" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="9">
-        <v>1</v>
-      </c>
-      <c r="J31" s="6"/>
+      <c r="I31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" ht="30">
-      <c r="B32" s="8">
+      <c r="B32" s="6">
         <v>5400</v>
       </c>
       <c r="C32" t="s">
@@ -1412,16 +1439,16 @@
       <c r="F32" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I32" s="9">
-        <v>1</v>
-      </c>
-      <c r="J32" s="6"/>
+      <c r="I32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="2:10">
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <v>5410</v>
       </c>
       <c r="C33" t="s">
@@ -1436,16 +1463,16 @@
       <c r="F33" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="9">
-        <v>1</v>
-      </c>
-      <c r="J33" s="6"/>
+      <c r="I33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="2:10" ht="30">
-      <c r="B34" s="8">
+      <c r="B34" s="6">
         <v>5420</v>
       </c>
       <c r="C34" t="s">
@@ -1460,18 +1487,18 @@
       <c r="F34" t="s">
         <v>36</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="9">
-        <v>0</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>86</v>
+      <c r="I34" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="30">
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <v>5500</v>
       </c>
       <c r="C35" t="s">
@@ -1486,16 +1513,16 @@
       <c r="F35" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I35" s="9">
-        <v>1</v>
-      </c>
-      <c r="J35" s="6"/>
+      <c r="I35" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="2:10" ht="30">
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <v>5510</v>
       </c>
       <c r="C36" t="s">
@@ -1510,22 +1537,22 @@
       <c r="F36" t="s">
         <v>74</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I36" s="9">
-        <v>1</v>
-      </c>
-      <c r="J36" s="6"/>
+      <c r="I36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="2:10">
-      <c r="G37" s="2"/>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" spans="2:10">
-      <c r="G38" s="2"/>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="G39" s="2"/>
+      <c r="G39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[ELAB-436] [ELAB-437] [ELAB-362] final work^1
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB699B83-3266-4EBB-8F69-4D26C8A27FDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0372534F-9FC6-45EE-90B6-9933FD9A27D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="88">
   <si>
     <t>Id</t>
   </si>
@@ -311,22 +311,13 @@
     <t>0%</t>
   </si>
   <si>
-    <t>70%</t>
-  </si>
-  <si>
     <t>75%</t>
   </si>
   <si>
     <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind (mindestens 60s) vorzuhalten und in dieser Zeit sind wiederholt (min. 3 mal) Verbindungsversuche zu unternehmen.</t>
   </si>
   <si>
-    <t>TODO: Beschreiben warum 0%</t>
-  </si>
-  <si>
-    <t>TODO: Beschreiben warum nur 75%</t>
-  </si>
-  <si>
-    <t>TODO: Beschreiben warum nur 70%</t>
+    <t>66%</t>
   </si>
 </sst>
 </file>
@@ -683,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1117,14 +1108,12 @@
         <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>89</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="45">
       <c r="B19" s="6">
@@ -1170,11 +1159,9 @@
         <v>40</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>90</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" ht="45">
       <c r="B21" s="6">
@@ -1354,9 +1341,7 @@
       <c r="I28" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" ht="30">
       <c r="B29" s="6">
@@ -1500,9 +1485,7 @@
       <c r="I34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J34" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="2:10" ht="30">
       <c r="B35" s="6">

</xml_diff>

<commit_message>
[ELAB-432] corrections and rewording of some parts^4
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4451D515-7EE8-4618-87AA-1E23BC6E1EBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479F06F6-CBB0-4E7A-9F8B-30B67FF0FA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -206,15 +206,9 @@
     <t>Beim ersten Aufruf des Frontends sind keine Session-Replay-Daten zu erheben.\par Stattdessen soll der Nutzer über einen Dialog auswählen können, ob er der Aufnahme zustimmt und erst danach sind diese Daten zu erheben.</t>
   </si>
   <si>
-    <t>Im Frontend sind Daten zwecks Session-Replay zu erheben, welche u. A. Benutzerinteraktionen, Schnittstellaufrufe sowie DOM-Manipulationen enthalten.</t>
-  </si>
-  <si>
     <t>Sämtlich erfasste Fehler des Frontends sind an ein "Error-Monitoring"-Partnersystem weiterzuleiten.</t>
   </si>
   <si>
-    <t>Tritt im Frontend ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, wenn ein Nutzer das Absenden eines Formular initiiert.</t>
-  </si>
-  <si>
     <t>Logmeldungen des Frontends sind an ein "Log-Management"-Partnersystem weiterzuleiten.\par Dabei sind Logmeldungen ab dem Log-Level "DEBUG" und höher zu übertragen.</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>Sämtlich erfasste Metriken des Frontends sind an ein "Metrik"-Partnersystem weiterzuleiten.</t>
   </si>
   <si>
-    <t>Sämtlich im Frontend erfasste Daten zum Session-Replay sind an ein "Session-Replay"-Partnersystem weiterzuleiten.</t>
-  </si>
-  <si>
     <t>Das Partnersystem, zu dem die Tracingdaten weitergeleitet werden, soll diese grafisch als Trace-Gantt-Diagramm darstellen können.</t>
   </si>
   <si>
@@ -245,9 +236,6 @@
     <t>Es existiert ein "Tracing"-Partnersystem, welches die Tracingdaten konsumiert und speichert. Zusammengehörige Spans sind zu Traces zusammenzufassen.</t>
   </si>
   <si>
-    <t>Die erfassten Tracingdaten sind für die Nutzer des Systems einsehbar, sowie können diese gefiltert werden. Die Filtierung erfolgt auf Basis von Eigenschaften der Tracingdaten (wie Name des meldenden Systems).</t>
-  </si>
-  <si>
     <t>Nutzer des Systems sollen die erfassten Fehler einsehen sowie diese filtern können. Die Filtierung erfolgt auf Basis der Eigenschaften der Fehler (bspw. der Fehlername).</t>
   </si>
   <si>
@@ -266,9 +254,6 @@
     <t>Bei Auftreten von bestimmten Fehlern oder einer Anzahl von Fehlern soll eine Meldung erzeugt werden können (per E-Mail, Slack, o. Ä.).</t>
   </si>
   <si>
-    <t>Es existiert ein "Session-Replay"-Partnersystem, zu die Daten zum Session-Replay gesendet werden und welches diese analysiert und speichert.</t>
-  </si>
-  <si>
     <t>Dieses System soll anhand der Daten jede aufgezeichnete Benutzersitzung in Videoform nachstellen.</t>
   </si>
   <si>
@@ -318,6 +303,21 @@
   </si>
   <si>
     <t>Im Frontend ist das Aufrufen von Schnittstellen mittels einer Logmeldung zu notieren. Hierbei soll vor Aufruf geloggt werden, welche Schnittstelle aufgerufen wird und mit welchen Parametern. Nach dem Aufruf soll bei Erfolg das Ergebnisobjekt geloggt werden, und bei einem Fehler ist dieser zu notieren.</t>
+  </si>
+  <si>
+    <t>Tritt im Frontend ein Use-Case auf, soll dieser im Log notiert werden. Beispielsweise soll notiert werden, wenn ein Nutzer das Absenden eines Formulars initiiert.</t>
+  </si>
+  <si>
+    <t>Im Frontend sind Daten zwecks Session-Replay zu erheben, welche u. A. Benutzerinteraktionen, Schnittstellenaufrufe sowie DOM-Manipulationen enthalten.</t>
+  </si>
+  <si>
+    <t>Sämtliche im Frontend erfasste Daten zum Session-Replay sind an ein "Session-Replay"-Partnersystem weiterzuleiten.</t>
+  </si>
+  <si>
+    <t>Die erfassten Tracingdaten sind für die Nutzer des Systems einsehbar und können gefiltert werden. Die Filtierung erfolgt auf Basis von Eigenschaften der Tracingdaten (wie Name des meldenden Systems).</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Session-Replay"-Partnersystem, zu dem die Daten zus Session-Replays gesendet werden und welches diese analysiert und speichert.</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -734,10 +734,10 @@
         <v>2110</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
@@ -746,11 +746,11 @@
         <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J3" s="5"/>
     </row>
@@ -759,10 +759,10 @@
         <v>2111</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>8</v>
@@ -771,11 +771,11 @@
         <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -784,10 +784,10 @@
         <v>2120</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
@@ -796,11 +796,11 @@
         <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -809,10 +809,10 @@
         <v>2210</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -834,10 +834,10 @@
         <v>2220</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>8</v>
@@ -846,11 +846,11 @@
         <v>22</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -859,10 +859,10 @@
         <v>2310</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>8</v>
@@ -875,7 +875,7 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -884,10 +884,10 @@
         <v>2311</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>15</v>
@@ -900,7 +900,7 @@
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -909,10 +909,10 @@
         <v>2320</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>8</v>
@@ -921,11 +921,11 @@
         <v>23</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -934,10 +934,10 @@
         <v>2410</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
@@ -946,11 +946,11 @@
         <v>19</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -959,10 +959,10 @@
         <v>2411</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -984,10 +984,10 @@
         <v>2420</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>8</v>
@@ -996,11 +996,11 @@
         <v>24</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1009,10 +1009,10 @@
         <v>2510</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>8</v>
@@ -1021,11 +1021,11 @@
         <v>20</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1034,10 +1034,10 @@
         <v>2511</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1059,10 +1059,10 @@
         <v>2520</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>8</v>
@@ -1071,11 +1071,11 @@
         <v>25</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1096,10 +1096,10 @@
         <v>3010</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1108,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1120,10 +1120,10 @@
         <v>3020</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1135,7 +1135,7 @@
         <v>38</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1144,10 +1144,10 @@
         <v>3100</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -1159,7 +1159,7 @@
         <v>40</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1168,10 +1168,10 @@
         <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1183,7 +1183,7 @@
         <v>41</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1204,10 +1204,10 @@
         <v>5100</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1216,10 +1216,10 @@
         <v>28</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1228,22 +1228,22 @@
         <v>5110</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1252,10 +1252,10 @@
         <v>5200</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1264,10 +1264,10 @@
         <v>29</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1276,22 +1276,22 @@
         <v>5210</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J26" s="5"/>
     </row>
@@ -1300,10 +1300,10 @@
         <v>5220</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1312,10 +1312,10 @@
         <v>30</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J27" s="5"/>
     </row>
@@ -1324,10 +1324,10 @@
         <v>5230</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -1336,10 +1336,10 @@
         <v>31</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J28" s="5"/>
     </row>
@@ -1348,10 +1348,10 @@
         <v>5300</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
@@ -1360,10 +1360,10 @@
         <v>32</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J29" s="5"/>
     </row>
@@ -1372,22 +1372,22 @@
         <v>5310</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J30" s="5"/>
     </row>
@@ -1396,10 +1396,10 @@
         <v>5320</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
@@ -1408,10 +1408,10 @@
         <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J31" s="5"/>
     </row>
@@ -1420,10 +1420,10 @@
         <v>5400</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
@@ -1432,10 +1432,10 @@
         <v>34</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1444,10 +1444,10 @@
         <v>5410</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
@@ -1456,10 +1456,10 @@
         <v>35</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J33" s="5"/>
     </row>
@@ -1468,10 +1468,10 @@
         <v>5420</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1480,10 +1480,10 @@
         <v>36</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J34" s="5"/>
     </row>
@@ -1492,10 +1492,10 @@
         <v>5500</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -1504,10 +1504,10 @@
         <v>37</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J35" s="5"/>
     </row>
@@ -1516,22 +1516,22 @@
         <v>5510</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="J36" s="5"/>
     </row>

</xml_diff>

<commit_message>
[ELAB-432] corrections and rewording of some parts^6
</commit_message>
<xml_diff>
--- a/data/anforderungsliste/Anforderungsliste.xlsx
+++ b/data/anforderungsliste/Anforderungsliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\anforderungsliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479F06F6-CBB0-4E7A-9F8B-30B67FF0FA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74D6721-5C7E-4531-A1D5-1FBE3693FF31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,12 +236,6 @@
     <t>Es existiert ein "Tracing"-Partnersystem, welches die Tracingdaten konsumiert und speichert. Zusammengehörige Spans sind zu Traces zusammenzufassen.</t>
   </si>
   <si>
-    <t>Nutzer des Systems sollen die erfassten Fehler einsehen sowie diese filtern können. Die Filtierung erfolgt auf Basis der Eigenschaften der Fehler (bspw. der Fehlername).</t>
-  </si>
-  <si>
-    <t>Nutzer des Systems sollen die erfassten Logmeldungen einsehen sowie diese filtern können. Die Filtierung erfolgt auf Basis der Eigenschaften der Logmeldung (bspw. des Log-Levels).</t>
-  </si>
-  <si>
     <t>Metriken sind grafisch darstellbar, bspw. in Histogrammen.</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>75%</t>
   </si>
   <si>
-    <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind (mindestens 60s) vorzuhalten und in dieser Zeit sind wiederholt (min. 3 mal) Verbindungsversuche zu unternehmen.</t>
-  </si>
-  <si>
     <t>66%</t>
   </si>
   <si>
@@ -314,10 +305,19 @@
     <t>Sämtliche im Frontend erfasste Daten zum Session-Replay sind an ein "Session-Replay"-Partnersystem weiterzuleiten.</t>
   </si>
   <si>
-    <t>Die erfassten Tracingdaten sind für die Nutzer des Systems einsehbar und können gefiltert werden. Die Filtierung erfolgt auf Basis von Eigenschaften der Tracingdaten (wie Name des meldenden Systems).</t>
-  </si>
-  <si>
-    <t>Es existiert ein "Session-Replay"-Partnersystem, zu dem die Daten zus Session-Replays gesendet werden und welches diese analysiert und speichert.</t>
+    <t>Nutzer des Systems sollen die erfassten Logmeldungen einsehen sowie diese filtern können. Die Filtrierung erfolgt auf Basis der Eigenschaften der Logmeldung (bspw. des Log-Levels).</t>
+  </si>
+  <si>
+    <t>Nutzer des Systems sollen die erfassten Fehler einsehen sowie diese filtern können. Die Filtrierung erfolgt auf Basis der Eigenschaften der Fehler (bspw. der Fehlername).</t>
+  </si>
+  <si>
+    <t>Die erfassten Tracingdaten sind für die Nutzer des Systems einsehbar und können gefiltert werden. Die Filtrierung erfolgt auf Basis von Eigenschaften der Tracingdaten (wie Name des meldenden Systems).</t>
+  </si>
+  <si>
+    <t>Es existiert ein "Session-Replay"-Partnersystem, zu dem die Daten des Session-Replays gesendet werden und welches diese analysiert und speichert.</t>
+  </si>
+  <si>
+    <t>Daten, die der Nachvollziehbarkeit dienen, sollen, wenn möglich, bei einer fehlgeschlagenen Verbindung nicht verworfen werden. Sie sind (mindestens 60s) vorzuhalten und in dieser Zeit sind wiederholt (min. 3-mal) Verbindungsversuche zu unternehmen.</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -734,10 +734,10 @@
         <v>2110</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
@@ -746,11 +746,11 @@
         <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J3" s="5"/>
     </row>
@@ -759,10 +759,10 @@
         <v>2111</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>8</v>
@@ -771,11 +771,11 @@
         <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -784,10 +784,10 @@
         <v>2120</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -809,10 +809,10 @@
         <v>2210</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
@@ -825,7 +825,7 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -834,10 +834,10 @@
         <v>2220</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>8</v>
@@ -850,7 +850,7 @@
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -859,10 +859,10 @@
         <v>2310</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>8</v>
@@ -875,7 +875,7 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -884,10 +884,10 @@
         <v>2311</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>15</v>
@@ -900,7 +900,7 @@
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -909,10 +909,10 @@
         <v>2320</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>8</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -934,10 +934,10 @@
         <v>2410</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
@@ -946,11 +946,11 @@
         <v>19</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -959,10 +959,10 @@
         <v>2411</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -984,10 +984,10 @@
         <v>2420</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>8</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1009,10 +1009,10 @@
         <v>2510</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>8</v>
@@ -1021,11 +1021,11 @@
         <v>20</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1034,10 +1034,10 @@
         <v>2511</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1059,10 +1059,10 @@
         <v>2520</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>8</v>
@@ -1071,11 +1071,11 @@
         <v>25</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1096,10 +1096,10 @@
         <v>3010</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1108,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1120,10 +1120,10 @@
         <v>3020</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1135,7 +1135,7 @@
         <v>38</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1144,10 +1144,10 @@
         <v>3100</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -1159,7 +1159,7 @@
         <v>40</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1168,10 +1168,10 @@
         <v>3200</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1183,7 +1183,7 @@
         <v>41</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1204,10 +1204,10 @@
         <v>5100</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -1219,7 +1219,7 @@
         <v>56</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1228,10 +1228,10 @@
         <v>5110</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -1240,10 +1240,10 @@
         <v>55</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1252,10 +1252,10 @@
         <v>5200</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1267,7 +1267,7 @@
         <v>57</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J25" s="5"/>
     </row>
@@ -1276,22 +1276,22 @@
         <v>5210</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J26" s="5"/>
     </row>
@@ -1300,10 +1300,10 @@
         <v>5220</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1315,7 +1315,7 @@
         <v>58</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J27" s="5"/>
     </row>
@@ -1324,10 +1324,10 @@
         <v>5230</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -1336,10 +1336,10 @@
         <v>31</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J28" s="5"/>
     </row>
@@ -1348,10 +1348,10 @@
         <v>5300</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
@@ -1363,7 +1363,7 @@
         <v>59</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J29" s="5"/>
     </row>
@@ -1372,22 +1372,22 @@
         <v>5310</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J30" s="5"/>
     </row>
@@ -1396,10 +1396,10 @@
         <v>5320</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
@@ -1411,7 +1411,7 @@
         <v>54</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J31" s="5"/>
     </row>
@@ -1420,10 +1420,10 @@
         <v>5400</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
@@ -1432,10 +1432,10 @@
         <v>34</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J32" s="5"/>
     </row>
@@ -1444,10 +1444,10 @@
         <v>5410</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
         <v>16</v>
@@ -1456,10 +1456,10 @@
         <v>35</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J33" s="5"/>
     </row>
@@ -1468,10 +1468,10 @@
         <v>5420</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1480,10 +1480,10 @@
         <v>36</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J34" s="5"/>
     </row>
@@ -1492,10 +1492,10 @@
         <v>5500</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -1504,10 +1504,10 @@
         <v>37</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J35" s="5"/>
     </row>
@@ -1516,22 +1516,22 @@
         <v>5510</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J36" s="5"/>
     </row>

</xml_diff>